<commit_message>
UPDATE: data imbalance good answer
</commit_message>
<xml_diff>
--- a/2025_07_02_OhLoRA_ML_Tutor/ai_quiz/dataset/question_list.xlsx
+++ b/2025_07_02_OhLoRA_ML_Tutor/ai_quiz/dataset/question_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B033463F-D670-4E91-9E46-F92BC31B0A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44B483A-4C4E-40AF-B186-7A649C0481C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2868" yWindow="132" windowWidth="27852" windowHeight="18468" xr2:uid="{07338742-8F51-42F9-A75F-1FCFBE7C4D0C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{07338742-8F51-42F9-A75F-1FCFBE7C4D0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -243,10 +243,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>데이터 불균형은 특정 Class 의 데이터가 다른 Class 의 데이터보다 훨씬 많은 등 각 Class 의 데이터 개수가 유의미하게 차이 나는 것이다. 이를 해결하기 위해서는 데이터를 새로 추가/제거하는 방법 (데이터 개수가 적은 Minority Class 데이터 추가 수집, Data Augmentation, Undersampling &amp; Oversampling), 학습 환경만 바꾸는 방법 (성능 평가 지표를 F1 Score, PR-AUC, ROC-AUC 등으로 선택, 데이터가 적은 Class 는 높은 가중치를 두는 등 가중치 조정) 이 있다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>차원의 저주</t>
     </r>
@@ -1374,6 +1370,10 @@
   </si>
   <si>
     <t>NLP|트랜스포머|상세 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 불균형은 특정 Class 의 데이터가 다른 Class 의 데이터보다 훨씬 많은 등 각 Class 의 데이터 개수가 유의미하게 차이 나는 것이다. 이를 해결하기 위해서는 데이터를 새로 추가/제거하는 방법 (데이터 개수가 적은 Minority Class 데이터 추가 수집, Data Augmentation, Undersampling &amp; Oversampling), 학습 환경만 바꾸는 방법 (성능 평가 지표를 F1 Score, PR-AUC, ROC-AUC 등으로 선택, 데이터가 적은 Class 는 손실 함수에서 높은 가중치를 두는 등 가중치 조정) 이 있다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1756,8 +1756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF56922-B03A-4496-8414-3644939C6218}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1786,7 +1786,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="104.4" x14ac:dyDescent="0.4">
@@ -1797,7 +1797,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
@@ -1808,7 +1808,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="104.4" x14ac:dyDescent="0.4">
@@ -1819,7 +1819,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
@@ -1830,7 +1830,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="121.8" x14ac:dyDescent="0.4">
@@ -1841,7 +1841,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
@@ -1852,7 +1852,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="87" x14ac:dyDescent="0.4">
@@ -1863,7 +1863,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
@@ -1874,7 +1874,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="104.4" x14ac:dyDescent="0.4">
@@ -1882,472 +1882,472 @@
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>157</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="156.6" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="121.8" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="121.8" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="C38" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="121.8" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="C39" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="139.19999999999999" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="C46" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="C47" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPDATE: L1, L2 regularization good answer
</commit_message>
<xml_diff>
--- a/2025_07_02_OhLoRA_ML_Tutor/ai_quiz/dataset/question_list.xlsx
+++ b/2025_07_02_OhLoRA_ML_Tutor/ai_quiz/dataset/question_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44B483A-4C4E-40AF-B186-7A649C0481C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF1FCB1-601F-455B-BC33-2BEA155B8832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{07338742-8F51-42F9-A75F-1FCFBE7C4D0C}"/>
   </bookViews>
@@ -950,10 +950,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Regularization (정규화) 는 오버피팅을 방지하기 위해 Loss Function 에 새로운 항을 추가하는 것을 말한다. L1 Regularization 은 weight 의 절댓값의 크기의 합에 일정 비율을 곱한 값을, L2 Regularization 은 weight 의 제곱의 합에 일정 비율을 곱한 값을 원래의 Loss Function 에 더하는 것이다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Batch Normalization 과 Layer Normalization 이란? 그리고 그 차이점은? </t>
     </r>
@@ -1374,6 +1370,10 @@
   </si>
   <si>
     <t>데이터 불균형은 특정 Class 의 데이터가 다른 Class 의 데이터보다 훨씬 많은 등 각 Class 의 데이터 개수가 유의미하게 차이 나는 것이다. 이를 해결하기 위해서는 데이터를 새로 추가/제거하는 방법 (데이터 개수가 적은 Minority Class 데이터 추가 수집, Data Augmentation, Undersampling &amp; Oversampling), 학습 환경만 바꾸는 방법 (성능 평가 지표를 F1 Score, PR-AUC, ROC-AUC 등으로 선택, 데이터가 적은 Class 는 손실 함수에서 높은 가중치를 두는 등 가중치 조정) 이 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Regularization (정규화) 는 오버피팅을 방지하기 위해 Loss Function 에 새로운 항을 추가하는 것을 말한다. L1 Regularization 은 weight 의 절댓값의 크기의 평균에 일정 비율을 곱한 값을, L2 Regularization 은 weight 의 제곱의 평균에 일정 비율을 곱한 값을 원래의 Loss Function 에 더하는 것이다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1756,8 +1756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF56922-B03A-4496-8414-3644939C6218}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1852,7 +1852,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="87" x14ac:dyDescent="0.4">
@@ -1882,7 +1882,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>34</v>
@@ -2160,7 +2160,7 @@
         <v>103</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
@@ -2179,175 +2179,175 @@
         <v>107</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="121.8" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="C39" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="139.19999999999999" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="C46" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="C47" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPDATE: batch & layer normalization good answer
</commit_message>
<xml_diff>
--- a/2025_07_02_OhLoRA_ML_Tutor/ai_quiz/dataset/question_list.xlsx
+++ b/2025_07_02_OhLoRA_ML_Tutor/ai_quiz/dataset/question_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF1FCB1-601F-455B-BC33-2BEA155B8832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F651D9A-8F7D-45D9-A45E-32DE83A235E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{07338742-8F51-42F9-A75F-1FCFBE7C4D0C}"/>
   </bookViews>
@@ -965,10 +965,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Batch Normalization (배치 정규화) 은 딥러닝의 특정 레이어에서, 1개의 batch 내의 데이터에 대해, 해당 레이어에서의 위치가 동일한 feature 값끼리 평균과 표준편차를 구해서 정규화하는 것이고, Layer Normalization 은 특정 레이어에서 각 sample 에 해당하는 모든 feature 값에 대해, 동일한 sample 에 해당하는 feature 값끼리 평균과 표준편차를 구해서 정규화하는 것이다. 즉 차이점은 Batch Normalization 은 레이어에서의 위치를 기준으로, Layer Normalization 은 속해 있는 sample 을 기준으로 그룹화하여 평균과 표준편차를 계산한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Transfer Learning (전이학습) 이 요즘 자주 쓰이고 있잖아! </t>
     </r>
@@ -1374,6 +1370,10 @@
   </si>
   <si>
     <t>Regularization (정규화) 는 오버피팅을 방지하기 위해 Loss Function 에 새로운 항을 추가하는 것을 말한다. L1 Regularization 은 weight 의 절댓값의 크기의 평균에 일정 비율을 곱한 값을, L2 Regularization 은 weight 의 제곱의 평균에 일정 비율을 곱한 값을 원래의 Loss Function 에 더하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Batch Normalization (배치 정규화) 은 딥러닝의 특정 레이어에서, 1개의 batch 내의 데이터에 대해, 해당 레이어에서의 신경망 내에서의 위치가 동일한 feature 값끼리 평균과 표준편차를 구해서 정규화하는 것이고, Layer Normalization 은 특정 레이어에서 각 sample 에 해당하는 모든 feature 값에 대해, 동일한 sample 에 해당하는 feature 값끼리 평균과 표준편차를 구해서 정규화하는 것이다. 즉 차이점은 Batch Normalization 은 레이어에서의 신경망 내에서의 위치를 기준으로, Layer Normalization 은 속해 있는 sample 을 기준으로 그룹화하여 평균과 표준편차를 계산한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1757,7 +1757,7 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1852,7 +1852,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="87" x14ac:dyDescent="0.4">
@@ -1882,7 +1882,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>34</v>
@@ -2160,7 +2160,7 @@
         <v>103</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
@@ -2179,10 +2179,10 @@
         <v>107</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="121.8" x14ac:dyDescent="0.4">
@@ -2190,164 +2190,164 @@
         <v>108</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="139.19999999999999" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="C46" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="C47" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="87" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>